<commit_message>
Nieuwe design kamers + Kostenberekening
</commit_message>
<xml_diff>
--- a/Logboek/Logboek technische progressie.xlsx
+++ b/Logboek/Logboek technische progressie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31613\Documents\Leerjaar 2\Periode 2.2\Radicale kunstspeeltuin\Logboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31613\Documents\Mediacollege Amsterdam\Leerjaar 2\Periode 2.2\Radicale kunstspeeltuin\Logboek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5476B8C6-8788-43EA-8BB3-F609240CFCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12666FC9-9AB5-4EC5-AF0E-62D2EAC86E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1667225-B0DF-4400-BBEA-B6543560BCC0}"/>
   </bookViews>
@@ -272,6 +272,33 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,33 +351,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,7 +697,7 @@
   <dimension ref="B2:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22:W25"/>
+      <selection activeCell="K18" sqref="K18:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,520 +785,520 @@
       <c r="W5" s="32"/>
     </row>
     <row r="6" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="12" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="14"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="23"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="17"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="26"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="17"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="26"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="20"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="29"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="12" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="14"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="23"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="17"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="26"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="17"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="26"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="20"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="29"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="12" t="s">
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="14"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="23"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="26"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="17"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="26"/>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="20"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="29"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="3" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="14"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="23"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="17"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="26"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="17"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="26"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="20"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="29"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="3" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="3" t="s">
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="14"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="23"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="17"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="26"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="17"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="26"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="20"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="29"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="N26" s="1"/>
@@ -1334,14 +1334,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B22:D25"/>
-    <mergeCell ref="E22:G25"/>
-    <mergeCell ref="H22:J25"/>
-    <mergeCell ref="K22:W25"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:W5"/>
     <mergeCell ref="B2:W3"/>
     <mergeCell ref="H18:J21"/>
     <mergeCell ref="K18:W21"/>
@@ -1358,6 +1350,14 @@
     <mergeCell ref="H14:J17"/>
     <mergeCell ref="K14:W17"/>
     <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B22:D25"/>
+    <mergeCell ref="E22:G25"/>
+    <mergeCell ref="H22:J25"/>
+    <mergeCell ref="K22:W25"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:W5"/>
     <mergeCell ref="E18:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>